<commit_message>
Added toy datasets for testing with NCDE and also NODE architectures
</commit_message>
<xml_diff>
--- a/Classification Results/Augmented Data/CORT ONLY VPOP Classification/By Diagnosis/CORT ONLY VPOP Classification Summary (Plus Ableson MDD 0 and 12).xlsx
+++ b/Classification Results/Augmented Data/CORT ONLY VPOP Classification/By Diagnosis/CORT ONLY VPOP Classification Summary (Plus Ableson MDD 0 and 12).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher/Documents/PTSD/NCDE Model/Classification Results/Augmented Data/CORT ONLY VPOP Classification/By Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E08CB3-1002-0142-B28F-740D56CF0432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBDC793-5584-1F44-88D6-5B7A63E4061A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="500" windowWidth="19400" windowHeight="16660" xr2:uid="{064A12D9-DF30-0A45-B172-879C6B680B9E}"/>
+    <workbookView xWindow="17740" yWindow="2680" windowWidth="19400" windowHeight="16660" xr2:uid="{064A12D9-DF30-0A45-B172-879C6B680B9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="17">
   <si>
     <t>Control</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>1, 4, 5, 7, 15</t>
+  </si>
+  <si>
+    <t>2000 Iterations</t>
   </si>
 </sst>
 </file>
@@ -289,13 +292,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -307,7 +307,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -634,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF02A33-AEE7-C74D-B125-3664DD3F27B5}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,16 +668,16 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -683,80 +686,107 @@
         <v>8</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="14"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>7</v>
+      </c>
       <c r="F5" s="4">
         <f>SUM(C5:E5)/30</f>
-        <v>0</v>
+        <v>0.43333333333333335</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="5">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5">
+        <v>3</v>
+      </c>
       <c r="F6" s="4">
         <f>SUM(C6:E6)/30</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="5">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5">
+        <v>6</v>
+      </c>
       <c r="F7" s="7">
         <f>SUM(C7:E7)/30</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="14">
-        <v>0</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="5">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1</v>
+      </c>
       <c r="F8" s="7">
         <f>SUM(C8:E8)/18</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="16"/>
+      <c r="A9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15"/>
       <c r="C9" s="7">
         <f>SUM(C5:C8)/36</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" ref="D9:E9" si="0">SUM(D5:D8)/36</f>
-        <v>0</v>
+        <v>0.47222222222222221</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.47222222222222221</v>
       </c>
       <c r="F9" s="10">
         <f>SUM(C5:E7)/87</f>
-        <v>0</v>
+        <v>0.40229885057471265</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -767,7 +797,7 @@
       </c>
       <c r="F10" s="7">
         <f>SUM(C5:E7)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -778,7 +808,7 @@
       </c>
       <c r="F11" s="7">
         <f>SUM(-F10, 108)</f>
-        <v>108</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -793,16 +823,16 @@
       <c r="B13" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -811,80 +841,107 @@
         <v>8</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="14"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="20"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
+      <c r="C15" s="4">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
       <c r="F15" s="4">
         <f>SUM(C15:E15)/30</f>
-        <v>0</v>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="5">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5">
+        <v>5</v>
+      </c>
       <c r="F16" s="4">
         <f>SUM(C16:E16)/30</f>
-        <v>0</v>
+        <v>0.36666666666666664</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="B17" s="12"/>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" s="5">
+        <v>6</v>
+      </c>
       <c r="F17" s="7">
         <f>SUM(C17:E17)/30</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="14">
-        <v>0</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
       <c r="F18" s="7">
         <f>SUM(C18:E18)/18</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="16"/>
+      <c r="A19" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="15"/>
       <c r="C19" s="7">
         <f>SUM(C15:C18)/36</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" ref="D19:E19" si="1">SUM(D15:D18)/36</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="F19" s="10">
         <f>SUM(C15:E17)/87</f>
-        <v>0</v>
+        <v>0.39080459770114945</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -895,7 +952,7 @@
       </c>
       <c r="F20" s="7">
         <f>SUM(C15:E17)</f>
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -906,174 +963,174 @@
       </c>
       <c r="F21" s="7">
         <f>SUM(-F20, 108)</f>
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="21" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
     </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-    </row>
-    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" t="s">
+    <row r="23" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C23" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D23" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>1</v>
-      </c>
+      <c r="F23" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="14"/>
+      <c r="A25" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="4">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>4</v>
+      </c>
+      <c r="E25" s="4">
+        <v>7</v>
+      </c>
+      <c r="F25" s="4">
+        <f>SUM(C25:E25)/30</f>
+        <v>0.46666666666666667</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="4">
-        <v>4</v>
-      </c>
-      <c r="D26" s="3">
-        <v>7</v>
-      </c>
-      <c r="E26" s="4">
-        <v>8</v>
+      <c r="A26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="5">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>3</v>
+      </c>
+      <c r="E26" s="5">
+        <v>4</v>
       </c>
       <c r="F26" s="4">
         <f>SUM(C26:E26)/30</f>
-        <v>0.6333333333333333</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="17"/>
+      <c r="A27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="12"/>
       <c r="C27" s="5">
         <v>2</v>
       </c>
-      <c r="D27">
-        <v>3</v>
+      <c r="D27" s="5">
+        <v>4</v>
       </c>
       <c r="E27" s="5">
-        <v>2</v>
-      </c>
-      <c r="F27" s="4">
+        <v>7</v>
+      </c>
+      <c r="F27" s="7">
         <f>SUM(C27:E27)/30</f>
-        <v>0.23333333333333334</v>
+        <v>0.43333333333333335</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" s="17"/>
+      <c r="A28" s="13">
+        <v>0</v>
+      </c>
+      <c r="B28" s="14"/>
       <c r="C28" s="5">
-        <v>4</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D28" s="5">
+        <v>3</v>
       </c>
       <c r="E28" s="5">
         <v>3</v>
       </c>
       <c r="F28" s="7">
-        <f>SUM(C28:E28)/30</f>
-        <v>0.4</v>
+        <f>SUM(C28:E28)/18</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="14">
-        <v>0</v>
+      <c r="A29" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="B29" s="15"/>
-      <c r="C29" s="5">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>4</v>
-      </c>
-      <c r="E29" s="5">
-        <v>3</v>
-      </c>
-      <c r="F29" s="7">
-        <f>SUM(C29:E29)/18</f>
-        <v>0.55555555555555558</v>
+      <c r="C29" s="7">
+        <f>SUM(C25:C28)/36</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D29" s="7">
+        <f t="shared" ref="D29:E29" si="2">SUM(D25:D28)/36</f>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="2"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F29" s="10">
+        <f>SUM(C25:E27)/87</f>
+        <v>0.41379310344827586</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="7">
-        <f>SUM(C26:C29)/36</f>
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="D30" s="7">
-        <f t="shared" ref="D30:E30" si="2">SUM(D26:D29)/36</f>
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="E30" s="7">
-        <f t="shared" si="2"/>
-        <v>0.44444444444444442</v>
-      </c>
-      <c r="F30" s="10">
-        <f>SUM(C26:E28)/87</f>
-        <v>0.43678160919540232</v>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="E30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F30" s="7">
+        <f>SUM(C25:E27)</f>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
-      <c r="E31" s="4" t="s">
-        <v>6</v>
+      <c r="E31" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="F31" s="7">
-        <f>SUM(C26:E28)</f>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="E32" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="7">
-        <f>SUM(-F31, 108)</f>
-        <v>70</v>
-      </c>
+        <f>SUM(-F30, 108)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
     </row>
     <row r="33" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -1083,16 +1140,16 @@
       <c r="B34" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="F34" s="11" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1101,10 +1158,10 @@
         <v>8</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="14"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
@@ -1112,62 +1169,62 @@
       </c>
       <c r="B36" s="20"/>
       <c r="C36" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E36" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F36" s="4">
         <f>SUM(C36:E36)/30</f>
-        <v>0.46666666666666667</v>
+        <v>0.6333333333333333</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="17"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="5">
         <v>2</v>
       </c>
       <c r="D37">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E37" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F37" s="4">
         <f>SUM(C37:E37)/30</f>
-        <v>0.43333333333333335</v>
+        <v>0.23333333333333334</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="17"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="5">
         <v>4</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E38" s="5">
         <v>3</v>
       </c>
       <c r="F38" s="7">
         <f>SUM(C38:E38)/30</f>
-        <v>0.36666666666666664</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="14">
+      <c r="A39" s="13">
         <v>0</v>
       </c>
-      <c r="B39" s="15"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="5">
         <v>3</v>
       </c>
@@ -1183,21 +1240,21 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="16"/>
+      <c r="A40" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="15"/>
       <c r="C40" s="7">
         <f>SUM(C36:C39)/36</f>
-        <v>0.33333333333333331</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="D40" s="7">
         <f t="shared" ref="D40:E40" si="3">SUM(D36:D39)/36</f>
-        <v>0.69444444444444442</v>
+        <v>0.52777777777777779</v>
       </c>
       <c r="E40" s="7">
         <f t="shared" si="3"/>
-        <v>0.30555555555555558</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="F40" s="10">
         <f>SUM(C36:E38)/87</f>
@@ -1228,332 +1285,882 @@
     </row>
     <row r="43" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="21" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
     </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-    </row>
-    <row r="45" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-      <c r="B45" t="s">
+    <row r="44" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C44" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D44" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="11" t="s">
+      <c r="E44" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F45" s="13" t="s">
-        <v>1</v>
-      </c>
+      <c r="F44" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="13"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="A46" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="4">
+        <v>3</v>
+      </c>
+      <c r="D46" s="3">
+        <v>9</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2</v>
+      </c>
+      <c r="F46" s="4">
+        <f>SUM(C46:E46)/30</f>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="12"/>
+      <c r="C47" s="5">
+        <v>2</v>
+      </c>
+      <c r="D47">
         <v>8</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="14"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
+      <c r="E47" s="5">
+        <v>3</v>
+      </c>
       <c r="F47" s="4">
         <f>SUM(C47:E47)/30</f>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="5">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48" s="5">
+        <v>3</v>
+      </c>
+      <c r="F48" s="7">
+        <f>SUM(C48:E48)/30</f>
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="4">
-        <f>SUM(C48:E48)/30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="5">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49" s="5">
+        <v>3</v>
+      </c>
       <c r="F49" s="7">
-        <f>SUM(C49:E49)/30</f>
-        <v>0</v>
+        <f>SUM(C49:E49)/18</f>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="14">
-        <v>0</v>
+      <c r="A50" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="B50" s="15"/>
-      <c r="C50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="7">
-        <f>SUM(C50:E50)/18</f>
-        <v>0</v>
+      <c r="C50" s="7">
+        <f>SUM(C46:C49)/36</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D50" s="7">
+        <f t="shared" ref="D50:E50" si="4">SUM(D46:D49)/36</f>
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="E50" s="7">
+        <f t="shared" si="4"/>
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="F50" s="10">
+        <f>SUM(C46:E48)/87</f>
+        <v>0.43678160919540232</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="7">
-        <f>SUM(C47:C50)/36</f>
-        <v>0</v>
-      </c>
-      <c r="D51" s="7">
-        <f t="shared" ref="D51:E51" si="4">SUM(D47:D50)/36</f>
-        <v>0</v>
-      </c>
-      <c r="E51" s="7">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F51" s="10">
-        <f>SUM(C47:E49)/87</f>
-        <v>0</v>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="E51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="7">
+        <f>SUM(C46:E48)</f>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="8"/>
       <c r="B52" s="8"/>
-      <c r="E52" s="4" t="s">
-        <v>6</v>
+      <c r="E52" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="F52" s="7">
-        <f>SUM(C47:E49)</f>
+        <f>SUM(-F51, 108)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A53" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+    </row>
+    <row r="54" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+      <c r="B54" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="E53" s="6" t="s">
+      <c r="C54" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="4">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3">
+        <v>4</v>
+      </c>
+      <c r="E56" s="4">
+        <v>8</v>
+      </c>
+      <c r="F56" s="4">
+        <f>SUM(C56:E56)/30</f>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="12"/>
+      <c r="C57" s="5">
+        <v>8</v>
+      </c>
+      <c r="D57" s="5">
+        <v>8</v>
+      </c>
+      <c r="E57" s="5">
         <v>7</v>
       </c>
-      <c r="F53" s="7">
-        <f>SUM(-F52, 108)</f>
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A54" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-    </row>
-    <row r="55" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="14"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4"/>
       <c r="F57" s="4">
         <f>SUM(C57:E57)/30</f>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="C58" s="5">
+        <v>4</v>
+      </c>
+      <c r="D58" s="5">
+        <v>4</v>
+      </c>
+      <c r="E58" s="5">
+        <v>3</v>
+      </c>
+      <c r="F58" s="7">
+        <f>SUM(C58:E58)/30</f>
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="4">
-        <f>SUM(C58:E58)/30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="5"/>
-      <c r="E59" s="5"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="5">
+        <v>3</v>
+      </c>
+      <c r="D59" s="5">
+        <v>4</v>
+      </c>
+      <c r="E59" s="5">
+        <v>3</v>
+      </c>
       <c r="F59" s="7">
-        <f>SUM(C59:E59)/30</f>
-        <v>0</v>
+        <f>SUM(C59:E59)/18</f>
+        <v>0.55555555555555558</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="14">
-        <v>0</v>
+      <c r="A60" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="B60" s="15"/>
-      <c r="C60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="7">
-        <f>SUM(C60:E60)/18</f>
-        <v>0</v>
+      <c r="C60" s="7">
+        <f>SUM(C56:C59)/36</f>
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="D60" s="7">
+        <f t="shared" ref="D60:E60" si="5">SUM(D56:D59)/36</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="5"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F60" s="10">
+        <f>SUM(C56:E58)/87</f>
+        <v>0.55172413793103448</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="7">
-        <f>SUM(C57:C60)/36</f>
-        <v>0</v>
-      </c>
-      <c r="D61" s="7">
-        <f t="shared" ref="D61:E61" si="5">SUM(D57:D60)/36</f>
-        <v>0</v>
-      </c>
-      <c r="E61" s="7">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F61" s="10">
-        <f>SUM(C57:E59)/87</f>
-        <v>0</v>
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="E61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" s="7">
+        <f>SUM(C56:E58)</f>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" s="7">
+        <f>SUM(-F61, 108)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A63" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+    </row>
+    <row r="64" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A64" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+    </row>
+    <row r="65" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+      <c r="B65" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="13"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="20"/>
+      <c r="C67" s="4">
+        <v>7</v>
+      </c>
+      <c r="D67" s="3">
+        <v>4</v>
+      </c>
+      <c r="E67" s="4">
+        <v>7</v>
+      </c>
+      <c r="F67" s="4">
+        <f>SUM(C67:E67)/30</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="12"/>
+      <c r="C68" s="5">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+      <c r="E68" s="5">
+        <v>4</v>
+      </c>
+      <c r="F68" s="4">
+        <f>SUM(C68:E68)/30</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" s="12"/>
+      <c r="C69" s="5">
+        <v>4</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69" s="5">
+        <v>2</v>
+      </c>
+      <c r="F69" s="7">
+        <f>SUM(C69:E69)/30</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="13">
+        <v>0</v>
+      </c>
+      <c r="B70" s="14"/>
+      <c r="C70" s="5">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+      <c r="E70" s="5">
+        <v>2</v>
+      </c>
+      <c r="F70" s="7">
+        <f>SUM(C70:E70)/18</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="15"/>
+      <c r="C71" s="7">
+        <f>SUM(C67:C70)/36</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D71" s="7">
+        <f t="shared" ref="D71:E71" si="6">SUM(D67:D70)/36</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E71" s="7">
+        <f t="shared" si="6"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F71" s="10">
+        <f>SUM(C67:E69)/87</f>
+        <v>0.41379310344827586</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="E72" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F62" s="7">
-        <f>SUM(C57:E59)</f>
+      <c r="F72" s="7">
+        <f>SUM(C67:E69)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="8"/>
+      <c r="B73" s="8"/>
+      <c r="E73" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" s="7">
+        <f>SUM(-F72, 108)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A74" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+    </row>
+    <row r="75" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+      <c r="B75" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="E63" s="6" t="s">
+      <c r="C75" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="13"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" s="20"/>
+      <c r="C77" s="4">
         <v>7</v>
       </c>
-      <c r="F63" s="7">
-        <f>SUM(-F62, 108)</f>
-        <v>108</v>
+      <c r="D77" s="3">
+        <v>4</v>
+      </c>
+      <c r="E77" s="4">
+        <v>7</v>
+      </c>
+      <c r="F77" s="4">
+        <f>SUM(C77:E77)/30</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="12"/>
+      <c r="C78" s="5">
+        <v>2</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+      <c r="E78" s="5">
+        <v>3</v>
+      </c>
+      <c r="F78" s="4">
+        <f>SUM(C78:E78)/30</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B79" s="12"/>
+      <c r="C79" s="5">
+        <v>4</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79" s="5">
+        <v>2</v>
+      </c>
+      <c r="F79" s="7">
+        <f>SUM(C79:E79)/30</f>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="13">
+        <v>0</v>
+      </c>
+      <c r="B80" s="14"/>
+      <c r="C80" s="5">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+      <c r="E80" s="5">
+        <v>3</v>
+      </c>
+      <c r="F80" s="7">
+        <f>SUM(C80:E80)/18</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="15"/>
+      <c r="C81" s="7">
+        <f>SUM(C77:C80)/36</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D81" s="7">
+        <f t="shared" ref="D81:E81" si="7">SUM(D77:D80)/36</f>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E81" s="7">
+        <f t="shared" si="7"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F81" s="10">
+        <f>SUM(C77:E79)/87</f>
+        <v>0.39080459770114945</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+      <c r="E82" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82" s="7">
+        <f>SUM(C77:E79)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
+      <c r="E83" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="7">
+        <f>SUM(-F82, 108)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+    </row>
+    <row r="85" spans="1:6" ht="26" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+      <c r="B85" t="s">
+        <v>0</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="17"/>
+      <c r="D86" s="17"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="13"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B87" s="20"/>
+      <c r="C87" s="4">
+        <v>7</v>
+      </c>
+      <c r="D87" s="3">
+        <v>8</v>
+      </c>
+      <c r="E87" s="4">
+        <v>8</v>
+      </c>
+      <c r="F87" s="4">
+        <f>SUM(C87:E87)/30</f>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" s="12"/>
+      <c r="C88" s="5">
+        <v>1</v>
+      </c>
+      <c r="D88" s="5">
+        <v>8</v>
+      </c>
+      <c r="E88" s="5">
+        <v>2</v>
+      </c>
+      <c r="F88" s="4">
+        <f>SUM(C88:E88)/30</f>
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B89" s="12"/>
+      <c r="C89" s="5">
+        <v>2</v>
+      </c>
+      <c r="D89" s="5">
+        <v>3</v>
+      </c>
+      <c r="E89" s="5">
+        <v>1</v>
+      </c>
+      <c r="F89" s="7">
+        <f>SUM(C89:E89)/30</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="13">
+        <v>0</v>
+      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="5">
+        <v>2</v>
+      </c>
+      <c r="D90" s="5">
+        <v>1</v>
+      </c>
+      <c r="E90" s="5">
+        <v>3</v>
+      </c>
+      <c r="F90" s="7">
+        <f>SUM(C90:E90)/18</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" s="15"/>
+      <c r="C91" s="7">
+        <f>SUM(C87:C90)/36</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D91" s="7">
+        <f t="shared" ref="D91:E91" si="8">SUM(D87:D90)/36</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E91" s="7">
+        <f t="shared" si="8"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="F91" s="10">
+        <f>SUM(C87:E89)/87</f>
+        <v>0.45977011494252873</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="8"/>
+      <c r="B92" s="8"/>
+      <c r="E92" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F92" s="7">
+        <f>SUM(C87:E89)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="8"/>
+      <c r="B93" s="8"/>
+      <c r="E93" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93" s="7">
+        <f>SUM(-F92, 108)</f>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="62">
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
+  <mergeCells count="92">
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A84:C84"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C23:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>